<commit_message>
Bugfix : conflit de type d'enseignement
</commit_message>
<xml_diff>
--- a/tables/Grille STI2D Soutenance V2016.xlsx
+++ b/tables/Grille STI2D Soutenance V2016.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>Poids de la compétence</t>
   </si>
@@ -230,9 +230,6 @@
   </si>
   <si>
     <t>Baccalauréat technologique "Sciences et technologies de l'Industrie et du Développement Durable"</t>
-  </si>
-  <si>
-    <t>3/3</t>
   </si>
   <si>
     <t>* La note est arrondie au demi-point  ou, si les examinateurs le souhaitent, au point supérieur</t>
@@ -457,6 +454,7 @@
       <sz val="10"/>
       <color indexed="10"/>
       <name val="Wingdings"/>
+      <charset val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -479,6 +477,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -503,6 +502,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -515,24 +515,28 @@
       <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1206,7 +1210,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1477,9 +1481,6 @@
     <xf numFmtId="12" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="21" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1579,6 +1580,92 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="42" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1658,92 +1745,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="22">
@@ -2111,585 +2112,585 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="21" style="85" customWidth="1"/>
-    <col min="2" max="2" width="96.5" style="85" customWidth="1"/>
-    <col min="3" max="3" width="3.875" style="85" customWidth="1"/>
-    <col min="4" max="256" width="11" style="85"/>
-    <col min="257" max="257" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="96.5" style="85" customWidth="1"/>
-    <col min="259" max="259" width="3.875" style="85" customWidth="1"/>
-    <col min="260" max="512" width="11" style="85"/>
-    <col min="513" max="513" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="96.5" style="85" customWidth="1"/>
-    <col min="515" max="515" width="3.875" style="85" customWidth="1"/>
-    <col min="516" max="768" width="11" style="85"/>
-    <col min="769" max="769" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="96.5" style="85" customWidth="1"/>
-    <col min="771" max="771" width="3.875" style="85" customWidth="1"/>
-    <col min="772" max="1024" width="11" style="85"/>
-    <col min="1025" max="1025" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="96.5" style="85" customWidth="1"/>
-    <col min="1027" max="1027" width="3.875" style="85" customWidth="1"/>
-    <col min="1028" max="1280" width="11" style="85"/>
-    <col min="1281" max="1281" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="96.5" style="85" customWidth="1"/>
-    <col min="1283" max="1283" width="3.875" style="85" customWidth="1"/>
-    <col min="1284" max="1536" width="11" style="85"/>
-    <col min="1537" max="1537" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="96.5" style="85" customWidth="1"/>
-    <col min="1539" max="1539" width="3.875" style="85" customWidth="1"/>
-    <col min="1540" max="1792" width="11" style="85"/>
-    <col min="1793" max="1793" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="96.5" style="85" customWidth="1"/>
-    <col min="1795" max="1795" width="3.875" style="85" customWidth="1"/>
-    <col min="1796" max="2048" width="11" style="85"/>
-    <col min="2049" max="2049" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="96.5" style="85" customWidth="1"/>
-    <col min="2051" max="2051" width="3.875" style="85" customWidth="1"/>
-    <col min="2052" max="2304" width="11" style="85"/>
-    <col min="2305" max="2305" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="96.5" style="85" customWidth="1"/>
-    <col min="2307" max="2307" width="3.875" style="85" customWidth="1"/>
-    <col min="2308" max="2560" width="11" style="85"/>
-    <col min="2561" max="2561" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="96.5" style="85" customWidth="1"/>
-    <col min="2563" max="2563" width="3.875" style="85" customWidth="1"/>
-    <col min="2564" max="2816" width="11" style="85"/>
-    <col min="2817" max="2817" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="96.5" style="85" customWidth="1"/>
-    <col min="2819" max="2819" width="3.875" style="85" customWidth="1"/>
-    <col min="2820" max="3072" width="11" style="85"/>
-    <col min="3073" max="3073" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="96.5" style="85" customWidth="1"/>
-    <col min="3075" max="3075" width="3.875" style="85" customWidth="1"/>
-    <col min="3076" max="3328" width="11" style="85"/>
-    <col min="3329" max="3329" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="96.5" style="85" customWidth="1"/>
-    <col min="3331" max="3331" width="3.875" style="85" customWidth="1"/>
-    <col min="3332" max="3584" width="11" style="85"/>
-    <col min="3585" max="3585" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="96.5" style="85" customWidth="1"/>
-    <col min="3587" max="3587" width="3.875" style="85" customWidth="1"/>
-    <col min="3588" max="3840" width="11" style="85"/>
-    <col min="3841" max="3841" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="96.5" style="85" customWidth="1"/>
-    <col min="3843" max="3843" width="3.875" style="85" customWidth="1"/>
-    <col min="3844" max="4096" width="11" style="85"/>
-    <col min="4097" max="4097" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="96.5" style="85" customWidth="1"/>
-    <col min="4099" max="4099" width="3.875" style="85" customWidth="1"/>
-    <col min="4100" max="4352" width="11" style="85"/>
-    <col min="4353" max="4353" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="96.5" style="85" customWidth="1"/>
-    <col min="4355" max="4355" width="3.875" style="85" customWidth="1"/>
-    <col min="4356" max="4608" width="11" style="85"/>
-    <col min="4609" max="4609" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="96.5" style="85" customWidth="1"/>
-    <col min="4611" max="4611" width="3.875" style="85" customWidth="1"/>
-    <col min="4612" max="4864" width="11" style="85"/>
-    <col min="4865" max="4865" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="96.5" style="85" customWidth="1"/>
-    <col min="4867" max="4867" width="3.875" style="85" customWidth="1"/>
-    <col min="4868" max="5120" width="11" style="85"/>
-    <col min="5121" max="5121" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="96.5" style="85" customWidth="1"/>
-    <col min="5123" max="5123" width="3.875" style="85" customWidth="1"/>
-    <col min="5124" max="5376" width="11" style="85"/>
-    <col min="5377" max="5377" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="96.5" style="85" customWidth="1"/>
-    <col min="5379" max="5379" width="3.875" style="85" customWidth="1"/>
-    <col min="5380" max="5632" width="11" style="85"/>
-    <col min="5633" max="5633" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="96.5" style="85" customWidth="1"/>
-    <col min="5635" max="5635" width="3.875" style="85" customWidth="1"/>
-    <col min="5636" max="5888" width="11" style="85"/>
-    <col min="5889" max="5889" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="96.5" style="85" customWidth="1"/>
-    <col min="5891" max="5891" width="3.875" style="85" customWidth="1"/>
-    <col min="5892" max="6144" width="11" style="85"/>
-    <col min="6145" max="6145" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="96.5" style="85" customWidth="1"/>
-    <col min="6147" max="6147" width="3.875" style="85" customWidth="1"/>
-    <col min="6148" max="6400" width="11" style="85"/>
-    <col min="6401" max="6401" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="96.5" style="85" customWidth="1"/>
-    <col min="6403" max="6403" width="3.875" style="85" customWidth="1"/>
-    <col min="6404" max="6656" width="11" style="85"/>
-    <col min="6657" max="6657" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="96.5" style="85" customWidth="1"/>
-    <col min="6659" max="6659" width="3.875" style="85" customWidth="1"/>
-    <col min="6660" max="6912" width="11" style="85"/>
-    <col min="6913" max="6913" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="96.5" style="85" customWidth="1"/>
-    <col min="6915" max="6915" width="3.875" style="85" customWidth="1"/>
-    <col min="6916" max="7168" width="11" style="85"/>
-    <col min="7169" max="7169" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="96.5" style="85" customWidth="1"/>
-    <col min="7171" max="7171" width="3.875" style="85" customWidth="1"/>
-    <col min="7172" max="7424" width="11" style="85"/>
-    <col min="7425" max="7425" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="96.5" style="85" customWidth="1"/>
-    <col min="7427" max="7427" width="3.875" style="85" customWidth="1"/>
-    <col min="7428" max="7680" width="11" style="85"/>
-    <col min="7681" max="7681" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="96.5" style="85" customWidth="1"/>
-    <col min="7683" max="7683" width="3.875" style="85" customWidth="1"/>
-    <col min="7684" max="7936" width="11" style="85"/>
-    <col min="7937" max="7937" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="96.5" style="85" customWidth="1"/>
-    <col min="7939" max="7939" width="3.875" style="85" customWidth="1"/>
-    <col min="7940" max="8192" width="11" style="85"/>
-    <col min="8193" max="8193" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="96.5" style="85" customWidth="1"/>
-    <col min="8195" max="8195" width="3.875" style="85" customWidth="1"/>
-    <col min="8196" max="8448" width="11" style="85"/>
-    <col min="8449" max="8449" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="96.5" style="85" customWidth="1"/>
-    <col min="8451" max="8451" width="3.875" style="85" customWidth="1"/>
-    <col min="8452" max="8704" width="11" style="85"/>
-    <col min="8705" max="8705" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="96.5" style="85" customWidth="1"/>
-    <col min="8707" max="8707" width="3.875" style="85" customWidth="1"/>
-    <col min="8708" max="8960" width="11" style="85"/>
-    <col min="8961" max="8961" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="96.5" style="85" customWidth="1"/>
-    <col min="8963" max="8963" width="3.875" style="85" customWidth="1"/>
-    <col min="8964" max="9216" width="11" style="85"/>
-    <col min="9217" max="9217" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="96.5" style="85" customWidth="1"/>
-    <col min="9219" max="9219" width="3.875" style="85" customWidth="1"/>
-    <col min="9220" max="9472" width="11" style="85"/>
-    <col min="9473" max="9473" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="96.5" style="85" customWidth="1"/>
-    <col min="9475" max="9475" width="3.875" style="85" customWidth="1"/>
-    <col min="9476" max="9728" width="11" style="85"/>
-    <col min="9729" max="9729" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="96.5" style="85" customWidth="1"/>
-    <col min="9731" max="9731" width="3.875" style="85" customWidth="1"/>
-    <col min="9732" max="9984" width="11" style="85"/>
-    <col min="9985" max="9985" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="96.5" style="85" customWidth="1"/>
-    <col min="9987" max="9987" width="3.875" style="85" customWidth="1"/>
-    <col min="9988" max="10240" width="11" style="85"/>
-    <col min="10241" max="10241" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="96.5" style="85" customWidth="1"/>
-    <col min="10243" max="10243" width="3.875" style="85" customWidth="1"/>
-    <col min="10244" max="10496" width="11" style="85"/>
-    <col min="10497" max="10497" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="96.5" style="85" customWidth="1"/>
-    <col min="10499" max="10499" width="3.875" style="85" customWidth="1"/>
-    <col min="10500" max="10752" width="11" style="85"/>
-    <col min="10753" max="10753" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="96.5" style="85" customWidth="1"/>
-    <col min="10755" max="10755" width="3.875" style="85" customWidth="1"/>
-    <col min="10756" max="11008" width="11" style="85"/>
-    <col min="11009" max="11009" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="96.5" style="85" customWidth="1"/>
-    <col min="11011" max="11011" width="3.875" style="85" customWidth="1"/>
-    <col min="11012" max="11264" width="11" style="85"/>
-    <col min="11265" max="11265" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="96.5" style="85" customWidth="1"/>
-    <col min="11267" max="11267" width="3.875" style="85" customWidth="1"/>
-    <col min="11268" max="11520" width="11" style="85"/>
-    <col min="11521" max="11521" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="96.5" style="85" customWidth="1"/>
-    <col min="11523" max="11523" width="3.875" style="85" customWidth="1"/>
-    <col min="11524" max="11776" width="11" style="85"/>
-    <col min="11777" max="11777" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="96.5" style="85" customWidth="1"/>
-    <col min="11779" max="11779" width="3.875" style="85" customWidth="1"/>
-    <col min="11780" max="12032" width="11" style="85"/>
-    <col min="12033" max="12033" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="96.5" style="85" customWidth="1"/>
-    <col min="12035" max="12035" width="3.875" style="85" customWidth="1"/>
-    <col min="12036" max="12288" width="11" style="85"/>
-    <col min="12289" max="12289" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="96.5" style="85" customWidth="1"/>
-    <col min="12291" max="12291" width="3.875" style="85" customWidth="1"/>
-    <col min="12292" max="12544" width="11" style="85"/>
-    <col min="12545" max="12545" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="96.5" style="85" customWidth="1"/>
-    <col min="12547" max="12547" width="3.875" style="85" customWidth="1"/>
-    <col min="12548" max="12800" width="11" style="85"/>
-    <col min="12801" max="12801" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="96.5" style="85" customWidth="1"/>
-    <col min="12803" max="12803" width="3.875" style="85" customWidth="1"/>
-    <col min="12804" max="13056" width="11" style="85"/>
-    <col min="13057" max="13057" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="96.5" style="85" customWidth="1"/>
-    <col min="13059" max="13059" width="3.875" style="85" customWidth="1"/>
-    <col min="13060" max="13312" width="11" style="85"/>
-    <col min="13313" max="13313" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="96.5" style="85" customWidth="1"/>
-    <col min="13315" max="13315" width="3.875" style="85" customWidth="1"/>
-    <col min="13316" max="13568" width="11" style="85"/>
-    <col min="13569" max="13569" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="96.5" style="85" customWidth="1"/>
-    <col min="13571" max="13571" width="3.875" style="85" customWidth="1"/>
-    <col min="13572" max="13824" width="11" style="85"/>
-    <col min="13825" max="13825" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="96.5" style="85" customWidth="1"/>
-    <col min="13827" max="13827" width="3.875" style="85" customWidth="1"/>
-    <col min="13828" max="14080" width="11" style="85"/>
-    <col min="14081" max="14081" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="96.5" style="85" customWidth="1"/>
-    <col min="14083" max="14083" width="3.875" style="85" customWidth="1"/>
-    <col min="14084" max="14336" width="11" style="85"/>
-    <col min="14337" max="14337" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="96.5" style="85" customWidth="1"/>
-    <col min="14339" max="14339" width="3.875" style="85" customWidth="1"/>
-    <col min="14340" max="14592" width="11" style="85"/>
-    <col min="14593" max="14593" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="96.5" style="85" customWidth="1"/>
-    <col min="14595" max="14595" width="3.875" style="85" customWidth="1"/>
-    <col min="14596" max="14848" width="11" style="85"/>
-    <col min="14849" max="14849" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="96.5" style="85" customWidth="1"/>
-    <col min="14851" max="14851" width="3.875" style="85" customWidth="1"/>
-    <col min="14852" max="15104" width="11" style="85"/>
-    <col min="15105" max="15105" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="96.5" style="85" customWidth="1"/>
-    <col min="15107" max="15107" width="3.875" style="85" customWidth="1"/>
-    <col min="15108" max="15360" width="11" style="85"/>
-    <col min="15361" max="15361" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="96.5" style="85" customWidth="1"/>
-    <col min="15363" max="15363" width="3.875" style="85" customWidth="1"/>
-    <col min="15364" max="15616" width="11" style="85"/>
-    <col min="15617" max="15617" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="96.5" style="85" customWidth="1"/>
-    <col min="15619" max="15619" width="3.875" style="85" customWidth="1"/>
-    <col min="15620" max="15872" width="11" style="85"/>
-    <col min="15873" max="15873" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="96.5" style="85" customWidth="1"/>
-    <col min="15875" max="15875" width="3.875" style="85" customWidth="1"/>
-    <col min="15876" max="16128" width="11" style="85"/>
-    <col min="16129" max="16129" width="16.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="96.5" style="85" customWidth="1"/>
-    <col min="16131" max="16131" width="3.875" style="85" customWidth="1"/>
-    <col min="16132" max="16384" width="11" style="85"/>
+    <col min="1" max="1" width="21" style="84" customWidth="1"/>
+    <col min="2" max="2" width="96.5" style="84" customWidth="1"/>
+    <col min="3" max="3" width="3.875" style="84" customWidth="1"/>
+    <col min="4" max="256" width="11" style="84"/>
+    <col min="257" max="257" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="96.5" style="84" customWidth="1"/>
+    <col min="259" max="259" width="3.875" style="84" customWidth="1"/>
+    <col min="260" max="512" width="11" style="84"/>
+    <col min="513" max="513" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="96.5" style="84" customWidth="1"/>
+    <col min="515" max="515" width="3.875" style="84" customWidth="1"/>
+    <col min="516" max="768" width="11" style="84"/>
+    <col min="769" max="769" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="96.5" style="84" customWidth="1"/>
+    <col min="771" max="771" width="3.875" style="84" customWidth="1"/>
+    <col min="772" max="1024" width="11" style="84"/>
+    <col min="1025" max="1025" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="96.5" style="84" customWidth="1"/>
+    <col min="1027" max="1027" width="3.875" style="84" customWidth="1"/>
+    <col min="1028" max="1280" width="11" style="84"/>
+    <col min="1281" max="1281" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="96.5" style="84" customWidth="1"/>
+    <col min="1283" max="1283" width="3.875" style="84" customWidth="1"/>
+    <col min="1284" max="1536" width="11" style="84"/>
+    <col min="1537" max="1537" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="96.5" style="84" customWidth="1"/>
+    <col min="1539" max="1539" width="3.875" style="84" customWidth="1"/>
+    <col min="1540" max="1792" width="11" style="84"/>
+    <col min="1793" max="1793" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="96.5" style="84" customWidth="1"/>
+    <col min="1795" max="1795" width="3.875" style="84" customWidth="1"/>
+    <col min="1796" max="2048" width="11" style="84"/>
+    <col min="2049" max="2049" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="96.5" style="84" customWidth="1"/>
+    <col min="2051" max="2051" width="3.875" style="84" customWidth="1"/>
+    <col min="2052" max="2304" width="11" style="84"/>
+    <col min="2305" max="2305" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="96.5" style="84" customWidth="1"/>
+    <col min="2307" max="2307" width="3.875" style="84" customWidth="1"/>
+    <col min="2308" max="2560" width="11" style="84"/>
+    <col min="2561" max="2561" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="96.5" style="84" customWidth="1"/>
+    <col min="2563" max="2563" width="3.875" style="84" customWidth="1"/>
+    <col min="2564" max="2816" width="11" style="84"/>
+    <col min="2817" max="2817" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="96.5" style="84" customWidth="1"/>
+    <col min="2819" max="2819" width="3.875" style="84" customWidth="1"/>
+    <col min="2820" max="3072" width="11" style="84"/>
+    <col min="3073" max="3073" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="96.5" style="84" customWidth="1"/>
+    <col min="3075" max="3075" width="3.875" style="84" customWidth="1"/>
+    <col min="3076" max="3328" width="11" style="84"/>
+    <col min="3329" max="3329" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="96.5" style="84" customWidth="1"/>
+    <col min="3331" max="3331" width="3.875" style="84" customWidth="1"/>
+    <col min="3332" max="3584" width="11" style="84"/>
+    <col min="3585" max="3585" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="96.5" style="84" customWidth="1"/>
+    <col min="3587" max="3587" width="3.875" style="84" customWidth="1"/>
+    <col min="3588" max="3840" width="11" style="84"/>
+    <col min="3841" max="3841" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="96.5" style="84" customWidth="1"/>
+    <col min="3843" max="3843" width="3.875" style="84" customWidth="1"/>
+    <col min="3844" max="4096" width="11" style="84"/>
+    <col min="4097" max="4097" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="96.5" style="84" customWidth="1"/>
+    <col min="4099" max="4099" width="3.875" style="84" customWidth="1"/>
+    <col min="4100" max="4352" width="11" style="84"/>
+    <col min="4353" max="4353" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="96.5" style="84" customWidth="1"/>
+    <col min="4355" max="4355" width="3.875" style="84" customWidth="1"/>
+    <col min="4356" max="4608" width="11" style="84"/>
+    <col min="4609" max="4609" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="96.5" style="84" customWidth="1"/>
+    <col min="4611" max="4611" width="3.875" style="84" customWidth="1"/>
+    <col min="4612" max="4864" width="11" style="84"/>
+    <col min="4865" max="4865" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="96.5" style="84" customWidth="1"/>
+    <col min="4867" max="4867" width="3.875" style="84" customWidth="1"/>
+    <col min="4868" max="5120" width="11" style="84"/>
+    <col min="5121" max="5121" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="96.5" style="84" customWidth="1"/>
+    <col min="5123" max="5123" width="3.875" style="84" customWidth="1"/>
+    <col min="5124" max="5376" width="11" style="84"/>
+    <col min="5377" max="5377" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="96.5" style="84" customWidth="1"/>
+    <col min="5379" max="5379" width="3.875" style="84" customWidth="1"/>
+    <col min="5380" max="5632" width="11" style="84"/>
+    <col min="5633" max="5633" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="96.5" style="84" customWidth="1"/>
+    <col min="5635" max="5635" width="3.875" style="84" customWidth="1"/>
+    <col min="5636" max="5888" width="11" style="84"/>
+    <col min="5889" max="5889" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="96.5" style="84" customWidth="1"/>
+    <col min="5891" max="5891" width="3.875" style="84" customWidth="1"/>
+    <col min="5892" max="6144" width="11" style="84"/>
+    <col min="6145" max="6145" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="96.5" style="84" customWidth="1"/>
+    <col min="6147" max="6147" width="3.875" style="84" customWidth="1"/>
+    <col min="6148" max="6400" width="11" style="84"/>
+    <col min="6401" max="6401" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="96.5" style="84" customWidth="1"/>
+    <col min="6403" max="6403" width="3.875" style="84" customWidth="1"/>
+    <col min="6404" max="6656" width="11" style="84"/>
+    <col min="6657" max="6657" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="96.5" style="84" customWidth="1"/>
+    <col min="6659" max="6659" width="3.875" style="84" customWidth="1"/>
+    <col min="6660" max="6912" width="11" style="84"/>
+    <col min="6913" max="6913" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="96.5" style="84" customWidth="1"/>
+    <col min="6915" max="6915" width="3.875" style="84" customWidth="1"/>
+    <col min="6916" max="7168" width="11" style="84"/>
+    <col min="7169" max="7169" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="96.5" style="84" customWidth="1"/>
+    <col min="7171" max="7171" width="3.875" style="84" customWidth="1"/>
+    <col min="7172" max="7424" width="11" style="84"/>
+    <col min="7425" max="7425" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="96.5" style="84" customWidth="1"/>
+    <col min="7427" max="7427" width="3.875" style="84" customWidth="1"/>
+    <col min="7428" max="7680" width="11" style="84"/>
+    <col min="7681" max="7681" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="96.5" style="84" customWidth="1"/>
+    <col min="7683" max="7683" width="3.875" style="84" customWidth="1"/>
+    <col min="7684" max="7936" width="11" style="84"/>
+    <col min="7937" max="7937" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="96.5" style="84" customWidth="1"/>
+    <col min="7939" max="7939" width="3.875" style="84" customWidth="1"/>
+    <col min="7940" max="8192" width="11" style="84"/>
+    <col min="8193" max="8193" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="96.5" style="84" customWidth="1"/>
+    <col min="8195" max="8195" width="3.875" style="84" customWidth="1"/>
+    <col min="8196" max="8448" width="11" style="84"/>
+    <col min="8449" max="8449" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="96.5" style="84" customWidth="1"/>
+    <col min="8451" max="8451" width="3.875" style="84" customWidth="1"/>
+    <col min="8452" max="8704" width="11" style="84"/>
+    <col min="8705" max="8705" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="96.5" style="84" customWidth="1"/>
+    <col min="8707" max="8707" width="3.875" style="84" customWidth="1"/>
+    <col min="8708" max="8960" width="11" style="84"/>
+    <col min="8961" max="8961" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="96.5" style="84" customWidth="1"/>
+    <col min="8963" max="8963" width="3.875" style="84" customWidth="1"/>
+    <col min="8964" max="9216" width="11" style="84"/>
+    <col min="9217" max="9217" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="96.5" style="84" customWidth="1"/>
+    <col min="9219" max="9219" width="3.875" style="84" customWidth="1"/>
+    <col min="9220" max="9472" width="11" style="84"/>
+    <col min="9473" max="9473" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="96.5" style="84" customWidth="1"/>
+    <col min="9475" max="9475" width="3.875" style="84" customWidth="1"/>
+    <col min="9476" max="9728" width="11" style="84"/>
+    <col min="9729" max="9729" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="96.5" style="84" customWidth="1"/>
+    <col min="9731" max="9731" width="3.875" style="84" customWidth="1"/>
+    <col min="9732" max="9984" width="11" style="84"/>
+    <col min="9985" max="9985" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="96.5" style="84" customWidth="1"/>
+    <col min="9987" max="9987" width="3.875" style="84" customWidth="1"/>
+    <col min="9988" max="10240" width="11" style="84"/>
+    <col min="10241" max="10241" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="96.5" style="84" customWidth="1"/>
+    <col min="10243" max="10243" width="3.875" style="84" customWidth="1"/>
+    <col min="10244" max="10496" width="11" style="84"/>
+    <col min="10497" max="10497" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="96.5" style="84" customWidth="1"/>
+    <col min="10499" max="10499" width="3.875" style="84" customWidth="1"/>
+    <col min="10500" max="10752" width="11" style="84"/>
+    <col min="10753" max="10753" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="96.5" style="84" customWidth="1"/>
+    <col min="10755" max="10755" width="3.875" style="84" customWidth="1"/>
+    <col min="10756" max="11008" width="11" style="84"/>
+    <col min="11009" max="11009" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="96.5" style="84" customWidth="1"/>
+    <col min="11011" max="11011" width="3.875" style="84" customWidth="1"/>
+    <col min="11012" max="11264" width="11" style="84"/>
+    <col min="11265" max="11265" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="96.5" style="84" customWidth="1"/>
+    <col min="11267" max="11267" width="3.875" style="84" customWidth="1"/>
+    <col min="11268" max="11520" width="11" style="84"/>
+    <col min="11521" max="11521" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="96.5" style="84" customWidth="1"/>
+    <col min="11523" max="11523" width="3.875" style="84" customWidth="1"/>
+    <col min="11524" max="11776" width="11" style="84"/>
+    <col min="11777" max="11777" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="96.5" style="84" customWidth="1"/>
+    <col min="11779" max="11779" width="3.875" style="84" customWidth="1"/>
+    <col min="11780" max="12032" width="11" style="84"/>
+    <col min="12033" max="12033" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="96.5" style="84" customWidth="1"/>
+    <col min="12035" max="12035" width="3.875" style="84" customWidth="1"/>
+    <col min="12036" max="12288" width="11" style="84"/>
+    <col min="12289" max="12289" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="96.5" style="84" customWidth="1"/>
+    <col min="12291" max="12291" width="3.875" style="84" customWidth="1"/>
+    <col min="12292" max="12544" width="11" style="84"/>
+    <col min="12545" max="12545" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="96.5" style="84" customWidth="1"/>
+    <col min="12547" max="12547" width="3.875" style="84" customWidth="1"/>
+    <col min="12548" max="12800" width="11" style="84"/>
+    <col min="12801" max="12801" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="96.5" style="84" customWidth="1"/>
+    <col min="12803" max="12803" width="3.875" style="84" customWidth="1"/>
+    <col min="12804" max="13056" width="11" style="84"/>
+    <col min="13057" max="13057" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="96.5" style="84" customWidth="1"/>
+    <col min="13059" max="13059" width="3.875" style="84" customWidth="1"/>
+    <col min="13060" max="13312" width="11" style="84"/>
+    <col min="13313" max="13313" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="96.5" style="84" customWidth="1"/>
+    <col min="13315" max="13315" width="3.875" style="84" customWidth="1"/>
+    <col min="13316" max="13568" width="11" style="84"/>
+    <col min="13569" max="13569" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="96.5" style="84" customWidth="1"/>
+    <col min="13571" max="13571" width="3.875" style="84" customWidth="1"/>
+    <col min="13572" max="13824" width="11" style="84"/>
+    <col min="13825" max="13825" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="96.5" style="84" customWidth="1"/>
+    <col min="13827" max="13827" width="3.875" style="84" customWidth="1"/>
+    <col min="13828" max="14080" width="11" style="84"/>
+    <col min="14081" max="14081" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="96.5" style="84" customWidth="1"/>
+    <col min="14083" max="14083" width="3.875" style="84" customWidth="1"/>
+    <col min="14084" max="14336" width="11" style="84"/>
+    <col min="14337" max="14337" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="96.5" style="84" customWidth="1"/>
+    <col min="14339" max="14339" width="3.875" style="84" customWidth="1"/>
+    <col min="14340" max="14592" width="11" style="84"/>
+    <col min="14593" max="14593" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="96.5" style="84" customWidth="1"/>
+    <col min="14595" max="14595" width="3.875" style="84" customWidth="1"/>
+    <col min="14596" max="14848" width="11" style="84"/>
+    <col min="14849" max="14849" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="96.5" style="84" customWidth="1"/>
+    <col min="14851" max="14851" width="3.875" style="84" customWidth="1"/>
+    <col min="14852" max="15104" width="11" style="84"/>
+    <col min="15105" max="15105" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="96.5" style="84" customWidth="1"/>
+    <col min="15107" max="15107" width="3.875" style="84" customWidth="1"/>
+    <col min="15108" max="15360" width="11" style="84"/>
+    <col min="15361" max="15361" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="96.5" style="84" customWidth="1"/>
+    <col min="15363" max="15363" width="3.875" style="84" customWidth="1"/>
+    <col min="15364" max="15616" width="11" style="84"/>
+    <col min="15617" max="15617" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="96.5" style="84" customWidth="1"/>
+    <col min="15619" max="15619" width="3.875" style="84" customWidth="1"/>
+    <col min="15620" max="15872" width="11" style="84"/>
+    <col min="15873" max="15873" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="96.5" style="84" customWidth="1"/>
+    <col min="15875" max="15875" width="3.875" style="84" customWidth="1"/>
+    <col min="15876" max="16128" width="11" style="84"/>
+    <col min="16129" max="16129" width="16.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="96.5" style="84" customWidth="1"/>
+    <col min="16131" max="16131" width="3.875" style="84" customWidth="1"/>
+    <col min="16132" max="16384" width="11" style="84"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickTop="1">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="106" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="107"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="108"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="86" t="s">
+      <c r="B2" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="87" t="s">
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="85" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="86" t="s">
+      <c r="B3" s="87" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="88" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="97" t="s">
+      <c r="B4" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="89" t="s">
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="96" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="97" t="s">
+      <c r="B5" s="89">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="90">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="97" t="s">
+      <c r="B6" s="90"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="91"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="97" t="s">
+      <c r="B7" s="90"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="91"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="97" t="s">
+      <c r="B8" s="91"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="92"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="97" t="s">
+      <c r="B9" s="91"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="92"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="97" t="s">
+      <c r="B10" s="92"/>
+    </row>
+    <row r="11" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A11" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="93"/>
-    </row>
-    <row r="11" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A11" s="98" t="s">
+      <c r="B11" s="93"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="102" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="108"/>
+    </row>
+    <row r="13" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A13" s="109" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="94"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="103" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="109"/>
-    </row>
-    <row r="13" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A13" s="110" t="s">
+      <c r="B13" s="110"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="111"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="103" t="s">
+      <c r="B14" s="108"/>
+      <c r="C14" s="94"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="111"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="94"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="111"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="94"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="111"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="94"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="111"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="94"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="111"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="94"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="111"/>
+      <c r="B20" s="112"/>
+      <c r="C20" s="94"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="111"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="94"/>
+    </row>
+    <row r="22" spans="1:9" ht="16.5" thickBot="1">
+      <c r="A22" s="113"/>
+      <c r="B22" s="114"/>
+      <c r="C22" s="94"/>
+    </row>
+    <row r="23" spans="1:9" s="95" customFormat="1">
+      <c r="A23" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="109"/>
-      <c r="C14" s="95"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="112"/>
-      <c r="B15" s="113"/>
-      <c r="C15" s="95"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="112"/>
-      <c r="B16" s="113"/>
-      <c r="C16" s="95"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="112"/>
-      <c r="B17" s="113"/>
-      <c r="C17" s="95"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="112"/>
-      <c r="B18" s="113"/>
-      <c r="C18" s="95"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="112"/>
-      <c r="B19" s="113"/>
-      <c r="C19" s="95"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="112"/>
-      <c r="B20" s="113"/>
-      <c r="C20" s="95"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="112"/>
-      <c r="B21" s="113"/>
-      <c r="C21" s="95"/>
-    </row>
-    <row r="22" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A22" s="114"/>
-      <c r="B22" s="115"/>
-      <c r="C22" s="95"/>
-    </row>
-    <row r="23" spans="1:9" s="96" customFormat="1">
-      <c r="A23" s="103" t="s">
+      <c r="B23" s="108"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="94"/>
+      <c r="H23" s="94"/>
+      <c r="I23" s="94"/>
+    </row>
+    <row r="24" spans="1:9" s="95" customFormat="1">
+      <c r="A24" s="98"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="94"/>
+      <c r="D24" s="94"/>
+      <c r="E24" s="94"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="94"/>
+      <c r="H24" s="94"/>
+      <c r="I24" s="94"/>
+    </row>
+    <row r="25" spans="1:9" s="95" customFormat="1">
+      <c r="A25" s="98"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="94"/>
+      <c r="G25" s="94"/>
+      <c r="H25" s="94"/>
+      <c r="I25" s="94"/>
+    </row>
+    <row r="26" spans="1:9" s="95" customFormat="1">
+      <c r="A26" s="98"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
+      <c r="E26" s="94"/>
+      <c r="F26" s="94"/>
+      <c r="G26" s="94"/>
+      <c r="H26" s="94"/>
+      <c r="I26" s="94"/>
+    </row>
+    <row r="27" spans="1:9" s="95" customFormat="1">
+      <c r="A27" s="98"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="94"/>
+      <c r="I27" s="94"/>
+    </row>
+    <row r="28" spans="1:9" s="95" customFormat="1">
+      <c r="A28" s="98"/>
+      <c r="B28" s="99"/>
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="94"/>
+      <c r="I28" s="94"/>
+    </row>
+    <row r="29" spans="1:9" s="95" customFormat="1">
+      <c r="A29" s="98"/>
+      <c r="B29" s="99"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="94"/>
+      <c r="I29" s="94"/>
+    </row>
+    <row r="30" spans="1:9" s="95" customFormat="1">
+      <c r="A30" s="98"/>
+      <c r="B30" s="99"/>
+      <c r="D30" s="94"/>
+      <c r="E30" s="94"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="94"/>
+      <c r="H30" s="94"/>
+      <c r="I30" s="94"/>
+    </row>
+    <row r="31" spans="1:9" s="95" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A31" s="100"/>
+      <c r="B31" s="101"/>
+      <c r="D31" s="94"/>
+      <c r="E31" s="94"/>
+      <c r="F31" s="94"/>
+      <c r="G31" s="94"/>
+      <c r="H31" s="94"/>
+      <c r="I31" s="94"/>
+    </row>
+    <row r="32" spans="1:9" s="95" customFormat="1">
+      <c r="A32" s="102" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="109"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="95"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="95"/>
-      <c r="I23" s="95"/>
-    </row>
-    <row r="24" spans="1:9" s="96" customFormat="1">
-      <c r="A24" s="99"/>
-      <c r="B24" s="100"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="95"/>
-      <c r="H24" s="95"/>
-      <c r="I24" s="95"/>
-    </row>
-    <row r="25" spans="1:9" s="96" customFormat="1">
-      <c r="A25" s="99"/>
-      <c r="B25" s="100"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="95"/>
-      <c r="I25" s="95"/>
-    </row>
-    <row r="26" spans="1:9" s="96" customFormat="1">
-      <c r="A26" s="99"/>
-      <c r="B26" s="100"/>
-      <c r="C26" s="95"/>
-      <c r="D26" s="95"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="95"/>
-      <c r="H26" s="95"/>
-      <c r="I26" s="95"/>
-    </row>
-    <row r="27" spans="1:9" s="96" customFormat="1">
-      <c r="A27" s="99"/>
-      <c r="B27" s="100"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="95"/>
-      <c r="I27" s="95"/>
-    </row>
-    <row r="28" spans="1:9" s="96" customFormat="1">
-      <c r="A28" s="99"/>
-      <c r="B28" s="100"/>
-      <c r="D28" s="95"/>
-      <c r="E28" s="95"/>
-      <c r="F28" s="95"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="95"/>
-      <c r="I28" s="95"/>
-    </row>
-    <row r="29" spans="1:9" s="96" customFormat="1">
-      <c r="A29" s="99"/>
-      <c r="B29" s="100"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="95"/>
-      <c r="F29" s="95"/>
-      <c r="G29" s="95"/>
-      <c r="H29" s="95"/>
-      <c r="I29" s="95"/>
-    </row>
-    <row r="30" spans="1:9" s="96" customFormat="1">
-      <c r="A30" s="99"/>
-      <c r="B30" s="100"/>
-      <c r="D30" s="95"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="95"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="95"/>
-      <c r="I30" s="95"/>
-    </row>
-    <row r="31" spans="1:9" s="96" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A31" s="101"/>
-      <c r="B31" s="102"/>
-      <c r="D31" s="95"/>
-      <c r="E31" s="95"/>
-      <c r="F31" s="95"/>
-      <c r="G31" s="95"/>
-      <c r="H31" s="95"/>
-      <c r="I31" s="95"/>
-    </row>
-    <row r="32" spans="1:9" s="96" customFormat="1">
-      <c r="A32" s="103" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="104"/>
-      <c r="D32" s="95"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="95"/>
-      <c r="G32" s="95"/>
-      <c r="H32" s="95"/>
-      <c r="I32" s="95"/>
-    </row>
-    <row r="33" spans="1:9" s="96" customFormat="1">
-      <c r="A33" s="99"/>
-      <c r="B33" s="100"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="95"/>
-      <c r="F33" s="95"/>
-      <c r="G33" s="95"/>
-      <c r="H33" s="95"/>
-      <c r="I33" s="95"/>
-    </row>
-    <row r="34" spans="1:9" s="96" customFormat="1">
-      <c r="A34" s="99"/>
-      <c r="B34" s="100"/>
-      <c r="D34" s="95"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
-      <c r="G34" s="95"/>
-      <c r="H34" s="95"/>
-      <c r="I34" s="95"/>
-    </row>
-    <row r="35" spans="1:9" s="96" customFormat="1">
-      <c r="A35" s="99"/>
-      <c r="B35" s="100"/>
-      <c r="D35" s="95"/>
-      <c r="E35" s="95"/>
-      <c r="F35" s="95"/>
-      <c r="G35" s="95"/>
-      <c r="H35" s="95"/>
-      <c r="I35" s="95"/>
-    </row>
-    <row r="36" spans="1:9" s="96" customFormat="1">
-      <c r="A36" s="99"/>
-      <c r="B36" s="100"/>
-      <c r="D36" s="95"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="95"/>
-      <c r="G36" s="95"/>
-      <c r="H36" s="95"/>
-      <c r="I36" s="95"/>
-    </row>
-    <row r="37" spans="1:9" s="96" customFormat="1">
-      <c r="A37" s="99"/>
-      <c r="B37" s="100"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="95"/>
-      <c r="F37" s="95"/>
-      <c r="G37" s="95"/>
-      <c r="H37" s="95"/>
-      <c r="I37" s="95"/>
-    </row>
-    <row r="38" spans="1:9" s="96" customFormat="1">
-      <c r="A38" s="99"/>
-      <c r="B38" s="100"/>
-      <c r="D38" s="95"/>
-      <c r="E38" s="95"/>
-      <c r="F38" s="95"/>
-      <c r="G38" s="95"/>
-      <c r="H38" s="95"/>
-      <c r="I38" s="95"/>
-    </row>
-    <row r="39" spans="1:9" s="96" customFormat="1">
-      <c r="A39" s="99"/>
-      <c r="B39" s="100"/>
-      <c r="D39" s="95"/>
-      <c r="E39" s="95"/>
-      <c r="F39" s="95"/>
-      <c r="G39" s="95"/>
-      <c r="H39" s="95"/>
-      <c r="I39" s="95"/>
-    </row>
-    <row r="40" spans="1:9" s="96" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A40" s="105"/>
-      <c r="B40" s="106"/>
-      <c r="D40" s="95"/>
-      <c r="E40" s="95"/>
-      <c r="F40" s="95"/>
-      <c r="G40" s="95"/>
-      <c r="H40" s="95"/>
-      <c r="I40" s="95"/>
+      <c r="B32" s="103"/>
+      <c r="D32" s="94"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="94"/>
+      <c r="H32" s="94"/>
+      <c r="I32" s="94"/>
+    </row>
+    <row r="33" spans="1:9" s="95" customFormat="1">
+      <c r="A33" s="98"/>
+      <c r="B33" s="99"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="94"/>
+      <c r="H33" s="94"/>
+      <c r="I33" s="94"/>
+    </row>
+    <row r="34" spans="1:9" s="95" customFormat="1">
+      <c r="A34" s="98"/>
+      <c r="B34" s="99"/>
+      <c r="D34" s="94"/>
+      <c r="E34" s="94"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="94"/>
+      <c r="H34" s="94"/>
+      <c r="I34" s="94"/>
+    </row>
+    <row r="35" spans="1:9" s="95" customFormat="1">
+      <c r="A35" s="98"/>
+      <c r="B35" s="99"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="94"/>
+      <c r="I35" s="94"/>
+    </row>
+    <row r="36" spans="1:9" s="95" customFormat="1">
+      <c r="A36" s="98"/>
+      <c r="B36" s="99"/>
+      <c r="D36" s="94"/>
+      <c r="E36" s="94"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="94"/>
+      <c r="H36" s="94"/>
+      <c r="I36" s="94"/>
+    </row>
+    <row r="37" spans="1:9" s="95" customFormat="1">
+      <c r="A37" s="98"/>
+      <c r="B37" s="99"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="94"/>
+      <c r="I37" s="94"/>
+    </row>
+    <row r="38" spans="1:9" s="95" customFormat="1">
+      <c r="A38" s="98"/>
+      <c r="B38" s="99"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="94"/>
+      <c r="G38" s="94"/>
+      <c r="H38" s="94"/>
+      <c r="I38" s="94"/>
+    </row>
+    <row r="39" spans="1:9" s="95" customFormat="1">
+      <c r="A39" s="98"/>
+      <c r="B39" s="99"/>
+      <c r="D39" s="94"/>
+      <c r="E39" s="94"/>
+      <c r="F39" s="94"/>
+      <c r="G39" s="94"/>
+      <c r="H39" s="94"/>
+      <c r="I39" s="94"/>
+    </row>
+    <row r="40" spans="1:9" s="95" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A40" s="104"/>
+      <c r="B40" s="105"/>
+      <c r="D40" s="94"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="94"/>
+      <c r="G40" s="94"/>
+      <c r="H40" s="94"/>
+      <c r="I40" s="94"/>
     </row>
     <row r="41" spans="1:9" ht="16.5" thickTop="1"/>
   </sheetData>
@@ -2716,7 +2717,7 @@
   <dimension ref="A1:Z38"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:L1"/>
+      <selection activeCell="E3" sqref="E3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75"/>
@@ -2753,10 +2754,10 @@
       <c r="H1" s="26"/>
       <c r="I1" s="63"/>
       <c r="J1" s="64"/>
-      <c r="K1" s="142" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="143"/>
+      <c r="K1" s="127" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" s="128"/>
       <c r="M1" s="67"/>
       <c r="N1" s="68"/>
     </row>
@@ -2764,11 +2765,11 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
       <c r="J2" s="65" t="s">
         <v>0</v>
       </c>
@@ -2788,10 +2789,10 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="13.5" thickBot="1">
-      <c r="A3" s="151" t="s">
+      <c r="A3" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="151"/>
+      <c r="B3" s="136"/>
       <c r="C3" s="13" t="s">
         <v>49</v>
       </c>
@@ -2799,14 +2800,17 @@
       <c r="E3" s="15">
         <v>0</v>
       </c>
-      <c r="F3" s="83">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G3" s="83">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="H3" s="84" t="s">
-        <v>53</v>
+      <c r="F3" s="83" t="str">
+        <f>"1/3"</f>
+        <v>1/3</v>
+      </c>
+      <c r="G3" s="83" t="str">
+        <f>"2/3"</f>
+        <v>2/3</v>
+      </c>
+      <c r="H3" s="83" t="str">
+        <f>"3/3"</f>
+        <v>3/3</v>
       </c>
       <c r="J3" s="52" t="s">
         <v>2</v>
@@ -2828,16 +2832,16 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="153"/>
-      <c r="C4" s="153"/>
-      <c r="D4" s="153"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="153"/>
-      <c r="G4" s="153"/>
-      <c r="H4" s="154"/>
+      <c r="B4" s="138"/>
+      <c r="C4" s="138"/>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="139"/>
       <c r="I4" s="16"/>
       <c r="J4" s="53">
         <v>0.2</v>
@@ -2860,16 +2864,16 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="15.95" customHeight="1">
-      <c r="A5" s="155" t="s">
+      <c r="A5" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="156" t="s">
+      <c r="B5" s="124" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="119"/>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="30"/>
@@ -2903,12 +2907,12 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="17.100000000000001" customHeight="1">
-      <c r="A6" s="155"/>
-      <c r="B6" s="156"/>
+      <c r="A6" s="115"/>
+      <c r="B6" s="124"/>
       <c r="C6" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="158"/>
+      <c r="D6" s="120"/>
       <c r="E6" s="33"/>
       <c r="F6" s="33"/>
       <c r="G6" s="33"/>
@@ -2951,7 +2955,7 @@
       <c r="C7" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="158"/>
+      <c r="D7" s="120"/>
       <c r="E7" s="69"/>
       <c r="F7" s="69"/>
       <c r="G7" s="69"/>
@@ -2985,16 +2989,16 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="147" t="s">
+      <c r="A8" s="132" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="148"/>
-      <c r="C8" s="148"/>
-      <c r="D8" s="148"/>
-      <c r="E8" s="148"/>
-      <c r="F8" s="148"/>
-      <c r="G8" s="148"/>
-      <c r="H8" s="149"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
+      <c r="H8" s="134"/>
       <c r="I8" s="16"/>
       <c r="J8" s="53">
         <v>0.15</v>
@@ -3017,16 +3021,16 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
-      <c r="A9" s="155" t="s">
+      <c r="A9" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="169" t="s">
+      <c r="B9" s="118" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="157"/>
+      <c r="D9" s="119"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
       <c r="G9" s="38"/>
@@ -3060,12 +3064,12 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
-      <c r="A10" s="155"/>
-      <c r="B10" s="169"/>
+      <c r="A10" s="115"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="164"/>
+      <c r="D10" s="140"/>
       <c r="E10" s="71"/>
       <c r="F10" s="71"/>
       <c r="G10" s="72"/>
@@ -3099,12 +3103,12 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
-      <c r="A11" s="155"/>
-      <c r="B11" s="169"/>
+      <c r="A11" s="115"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="158"/>
+      <c r="D11" s="120"/>
       <c r="E11" s="76"/>
       <c r="F11" s="76"/>
       <c r="G11" s="77"/>
@@ -3138,16 +3142,16 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="18" customHeight="1">
-      <c r="A12" s="155" t="s">
+      <c r="A12" s="115" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="156" t="s">
+      <c r="B12" s="124" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="158"/>
+      <c r="D12" s="120"/>
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
       <c r="G12" s="40"/>
@@ -3181,12 +3185,12 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="18" customHeight="1" thickBot="1">
-      <c r="A13" s="160"/>
-      <c r="B13" s="159"/>
+      <c r="A13" s="125"/>
+      <c r="B13" s="126"/>
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="165"/>
+      <c r="D13" s="141"/>
       <c r="E13" s="43"/>
       <c r="F13" s="43"/>
       <c r="G13" s="43"/>
@@ -3220,16 +3224,16 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="161" t="s">
+      <c r="A14" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="162"/>
-      <c r="C14" s="162"/>
-      <c r="D14" s="162"/>
-      <c r="E14" s="162"/>
-      <c r="F14" s="162"/>
-      <c r="G14" s="162"/>
-      <c r="H14" s="163"/>
+      <c r="B14" s="122"/>
+      <c r="C14" s="122"/>
+      <c r="D14" s="122"/>
+      <c r="E14" s="122"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="122"/>
+      <c r="H14" s="123"/>
       <c r="I14" s="16"/>
       <c r="J14" s="53">
         <v>0.45</v>
@@ -3261,7 +3265,7 @@
       <c r="C15" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="157"/>
+      <c r="D15" s="119"/>
       <c r="E15" s="40"/>
       <c r="F15" s="40"/>
       <c r="G15" s="40"/>
@@ -3304,7 +3308,7 @@
       <c r="C16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="158"/>
+      <c r="D16" s="120"/>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
@@ -3338,16 +3342,16 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" ht="18.95" customHeight="1">
-      <c r="A17" s="155" t="s">
+      <c r="A17" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="156" t="s">
+      <c r="B17" s="124" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="158"/>
+      <c r="D17" s="120"/>
       <c r="E17" s="74"/>
       <c r="F17" s="74"/>
       <c r="G17" s="74"/>
@@ -3381,12 +3385,12 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A18" s="160"/>
-      <c r="B18" s="159"/>
+      <c r="A18" s="125"/>
+      <c r="B18" s="126"/>
       <c r="C18" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="166"/>
+      <c r="D18" s="142"/>
       <c r="E18" s="79"/>
       <c r="F18" s="79"/>
       <c r="G18" s="79"/>
@@ -3420,16 +3424,16 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="161" t="s">
+      <c r="A19" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="162"/>
-      <c r="C19" s="162"/>
-      <c r="D19" s="162"/>
-      <c r="E19" s="162"/>
-      <c r="F19" s="162"/>
-      <c r="G19" s="162"/>
-      <c r="H19" s="163"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="122"/>
+      <c r="G19" s="122"/>
+      <c r="H19" s="123"/>
       <c r="I19" s="16"/>
       <c r="J19" s="53">
         <v>0.2</v>
@@ -3452,16 +3456,16 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" ht="25.5">
-      <c r="A20" s="155" t="s">
+      <c r="A20" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="156" t="s">
+      <c r="B20" s="124" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="157"/>
+      <c r="D20" s="119"/>
       <c r="E20" s="40"/>
       <c r="F20" s="40"/>
       <c r="G20" s="40"/>
@@ -3495,12 +3499,12 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" ht="14.1" customHeight="1">
-      <c r="A21" s="155"/>
-      <c r="B21" s="156"/>
+      <c r="A21" s="115"/>
+      <c r="B21" s="124"/>
       <c r="C21" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="158"/>
+      <c r="D21" s="120"/>
       <c r="E21" s="37"/>
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
@@ -3535,10 +3539,10 @@
     </row>
     <row r="22" spans="1:26">
       <c r="C22" s="17"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
-      <c r="G22" s="146"/>
-      <c r="H22" s="146"/>
+      <c r="E22" s="131"/>
+      <c r="F22" s="131"/>
+      <c r="G22" s="131"/>
+      <c r="H22" s="131"/>
       <c r="J22" s="19">
         <f>J4+J8+J19+J14</f>
         <v>1</v>
@@ -3564,15 +3568,15 @@
       <c r="C23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="144" t="str">
+      <c r="E23" s="129" t="str">
         <f>IF(M22&lt;&gt;1,"",L4+L8+L14+L19)</f>
         <v/>
       </c>
-      <c r="F23" s="144"/>
-      <c r="G23" s="145" t="s">
+      <c r="F23" s="129"/>
+      <c r="G23" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="145"/>
+      <c r="H23" s="130"/>
       <c r="I23" s="20"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -3591,16 +3595,16 @@
       <c r="C24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="128"/>
-      <c r="F24" s="129"/>
-      <c r="G24" s="130" t="s">
+      <c r="E24" s="155"/>
+      <c r="F24" s="156"/>
+      <c r="G24" s="157" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="131"/>
-      <c r="K24" s="116" t="s">
+      <c r="H24" s="158"/>
+      <c r="K24" s="143" t="s">
         <v>43</v>
       </c>
-      <c r="L24" s="117"/>
+      <c r="L24" s="144"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -3618,18 +3622,18 @@
       <c r="C25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="132">
+      <c r="E25" s="159">
         <f>E24*6</f>
         <v>0</v>
       </c>
-      <c r="F25" s="133"/>
-      <c r="G25" s="134">
+      <c r="F25" s="160"/>
+      <c r="G25" s="161">
         <v>120</v>
       </c>
-      <c r="H25" s="135"/>
+      <c r="H25" s="162"/>
       <c r="I25" s="16"/>
-      <c r="K25" s="118"/>
-      <c r="L25" s="119"/>
+      <c r="K25" s="145"/>
+      <c r="L25" s="146"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -3644,16 +3648,16 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26">
-      <c r="A26" s="125" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="125"/>
-      <c r="C26" s="125"/>
-      <c r="D26" s="125"/>
-      <c r="E26" s="125"/>
-      <c r="F26" s="125"/>
-      <c r="G26" s="125"/>
-      <c r="H26" s="125"/>
+      <c r="A26" s="152" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="152"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="152"/>
+      <c r="G26" s="152"/>
+      <c r="H26" s="152"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -3668,16 +3672,16 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" ht="13.5" thickBot="1">
-      <c r="A27" s="120" t="s">
+      <c r="A27" s="147" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="121"/>
-      <c r="C27" s="121"/>
-      <c r="D27" s="121"/>
-      <c r="E27" s="121"/>
-      <c r="F27" s="121"/>
-      <c r="G27" s="121"/>
-      <c r="H27" s="121"/>
+      <c r="B27" s="148"/>
+      <c r="C27" s="148"/>
+      <c r="D27" s="148"/>
+      <c r="E27" s="148"/>
+      <c r="F27" s="148"/>
+      <c r="G27" s="148"/>
+      <c r="H27" s="148"/>
       <c r="I27" s="21" t="s">
         <v>20</v>
       </c>
@@ -3695,18 +3699,18 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="167" t="s">
+      <c r="A28" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="168"/>
-      <c r="C28" s="122" t="s">
+      <c r="B28" s="117"/>
+      <c r="C28" s="149" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="123"/>
-      <c r="E28" s="123"/>
-      <c r="F28" s="123"/>
-      <c r="G28" s="123"/>
-      <c r="H28" s="124"/>
+      <c r="D28" s="150"/>
+      <c r="E28" s="150"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="150"/>
+      <c r="H28" s="151"/>
       <c r="I28" s="22"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
@@ -3722,14 +3726,14 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" ht="27.95" customHeight="1">
-      <c r="A29" s="138"/>
-      <c r="B29" s="139"/>
-      <c r="C29" s="139"/>
-      <c r="D29" s="139"/>
-      <c r="E29" s="139"/>
-      <c r="F29" s="139"/>
-      <c r="G29" s="139"/>
-      <c r="H29" s="140"/>
+      <c r="A29" s="165"/>
+      <c r="B29" s="166"/>
+      <c r="C29" s="166"/>
+      <c r="D29" s="166"/>
+      <c r="E29" s="166"/>
+      <c r="F29" s="166"/>
+      <c r="G29" s="166"/>
+      <c r="H29" s="167"/>
       <c r="I29" s="23"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
@@ -3745,14 +3749,14 @@
       <c r="Z29" s="3"/>
     </row>
     <row r="30" spans="1:26" ht="27.95" customHeight="1" thickBot="1">
-      <c r="A30" s="138"/>
-      <c r="B30" s="139"/>
-      <c r="C30" s="139"/>
-      <c r="D30" s="139"/>
-      <c r="E30" s="139"/>
-      <c r="F30" s="139"/>
-      <c r="G30" s="139"/>
-      <c r="H30" s="140"/>
+      <c r="A30" s="165"/>
+      <c r="B30" s="166"/>
+      <c r="C30" s="166"/>
+      <c r="D30" s="166"/>
+      <c r="E30" s="166"/>
+      <c r="F30" s="166"/>
+      <c r="G30" s="166"/>
+      <c r="H30" s="167"/>
       <c r="I30" s="23"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -3772,20 +3776,20 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31" spans="1:26" ht="27.95" customHeight="1" thickBot="1">
-      <c r="A31" s="136"/>
-      <c r="B31" s="137"/>
-      <c r="C31" s="137"/>
-      <c r="D31" s="137"/>
-      <c r="E31" s="137"/>
-      <c r="F31" s="137"/>
-      <c r="G31" s="137"/>
-      <c r="H31" s="141"/>
+      <c r="A31" s="163"/>
+      <c r="B31" s="164"/>
+      <c r="C31" s="164"/>
+      <c r="D31" s="164"/>
+      <c r="E31" s="164"/>
+      <c r="F31" s="164"/>
+      <c r="G31" s="164"/>
+      <c r="H31" s="168"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="126" t="s">
+      <c r="K31" s="153" t="s">
         <v>41</v>
       </c>
-      <c r="L31" s="127"/>
+      <c r="L31" s="154"/>
       <c r="N31" s="56"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
@@ -3951,15 +3955,19 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="K24:L25"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C29:H31"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="G23:H23"/>
@@ -3976,19 +3984,15 @@
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="D9:D13"/>
     <mergeCell ref="D15:D18"/>
-    <mergeCell ref="K24:L25"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C29:H31"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>